<commit_message>
Added const lec 30 files
</commit_message>
<xml_diff>
--- a/Complete DSA Notes/FINAL450.xlsx
+++ b/Complete DSA Notes/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bablove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\DSA\Complete DSA Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9E80F3-81F9-4735-907B-676F3073F90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1559,9 +1559,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1599,7 +1599,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1705,7 +1705,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1847,7 +1847,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,18 +1857,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26">
+    <row r="1" spans="1:3" ht="24.6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>